<commit_message>
success change data and store in .xlsx
</commit_message>
<xml_diff>
--- a/MySurvivorsGame/Assets/StreamingAssets/RealTimePlayerData.xlsx
+++ b/MySurvivorsGame/Assets/StreamingAssets/RealTimePlayerData.xlsx
@@ -5,13 +5,12 @@
   <sheets>
     <sheet state="visible" name="RealTimePlayerData" sheetId="1" r:id="rId4"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Speed</t>
   </si>
@@ -34,6 +33,9 @@
     <t>SoulNumber</t>
   </si>
   <si>
+    <t>ChooseDevil</t>
+  </si>
+  <si>
     <t>玩家速度</t>
   </si>
   <si>
@@ -55,19 +57,29 @@
     <t>靈魂數</t>
   </si>
   <si>
+    <t>玩家選擇的魔王</t>
+  </si>
+  <si>
     <t>float</t>
   </si>
   <si>
     <t>int</t>
+  </si>
+  <si>
+    <t>string</t>
+  </si>
+  <si>
+    <t>BoneMan</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <numFmts count="0"/>
   <fonts count="3">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
@@ -97,34 +109,32 @@
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1"/>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="1" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="left" vertical="bottom"/>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="2" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1"/>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="1" applyFont="1" fillId="2" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -322,10 +332,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -353,77 +364,89 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="H1" s="2" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>15</v>
+        <v>17</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1">
-        <v>2.0</v>
+        <v>0.5</v>
       </c>
       <c r="B4" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="C4" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="D4" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="E4" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="F4" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G4" s="1">
-        <v>0.0</v>
+        <v>0</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add CharacterManager.cs, Instantiate Devil Func
</commit_message>
<xml_diff>
--- a/MySurvivorsGame/Assets/StreamingAssets/RealTimePlayerData.xlsx
+++ b/MySurvivorsGame/Assets/StreamingAssets/RealTimePlayerData.xlsx
@@ -69,7 +69,7 @@
     <t>string</t>
   </si>
   <si>
-    <t>BoneMan</t>
+    <t>Reaper</t>
   </si>
 </sst>
 </file>
@@ -422,7 +422,7 @@
     </row>
     <row r="4">
       <c r="A4" s="1">
-        <v>0.5</v>
+        <v>2</v>
       </c>
       <c r="B4" s="1">
         <v>0</v>

</xml_diff>

<commit_message>
update playermove by data
</commit_message>
<xml_diff>
--- a/MySurvivorsGame/Assets/StreamingAssets/RealTimePlayerData.xlsx
+++ b/MySurvivorsGame/Assets/StreamingAssets/RealTimePlayerData.xlsx
@@ -5,13 +5,12 @@
   <sheets>
     <sheet state="visible" name="RealTimePlayerData" sheetId="1" r:id="rId4"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Speed</t>
   </si>
@@ -86,9 +85,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <numFmts count="0"/>
   <fonts count="3">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
@@ -118,37 +118,35 @@
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1"/>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="1" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" vertical="bottom"/>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="1" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="left" vertical="bottom"/>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="2" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1"/>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="1" applyFont="1" fillId="2" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -346,16 +344,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="9" max="9" width="31.13"/>
+    <col min="9" max="9" width="31.13" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -447,25 +446,25 @@
     </row>
     <row r="4">
       <c r="A4" s="1">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="B4" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="C4" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="D4" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="E4" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="F4" s="1">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="G4" s="1">
-        <v>0.0</v>
+        <v>0</v>
       </c>
       <c r="H4" s="3" t="s">
         <v>21</v>
@@ -475,6 +474,6 @@
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
change RealTimePlayerSata data type
</commit_message>
<xml_diff>
--- a/MySurvivorsGame/Assets/StreamingAssets/RealTimePlayerData.xlsx
+++ b/MySurvivorsGame/Assets/StreamingAssets/RealTimePlayerData.xlsx
@@ -10,12 +10,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+  <si>
+    <t>DevilName</t>
+  </si>
+  <si>
+    <t>Attack</t>
+  </si>
+  <si>
+    <t>HP</t>
+  </si>
   <si>
     <t>Speed</t>
   </si>
   <si>
-    <t>Exp</t>
+    <t>ExpEffect</t>
   </si>
   <si>
     <t>AbsorbExpRange</t>
@@ -30,19 +39,22 @@
     <t>DropRate</t>
   </si>
   <si>
-    <t>SoulNumber</t>
-  </si>
-  <si>
-    <t>ChooseDevil</t>
-  </si>
-  <si>
     <t>PrefabPath</t>
   </si>
   <si>
-    <t>玩家速度</t>
-  </si>
-  <si>
-    <t>經驗值</t>
+    <t>惡魔名稱</t>
+  </si>
+  <si>
+    <t>攻擊力</t>
+  </si>
+  <si>
+    <t>血量</t>
+  </si>
+  <si>
+    <t>速度</t>
+  </si>
+  <si>
+    <t>經驗值成長效率</t>
   </si>
   <si>
     <t>吸收經驗範圍</t>
@@ -57,22 +69,13 @@
     <t>寶箱掉落率</t>
   </si>
   <si>
-    <t>靈魂數</t>
-  </si>
-  <si>
-    <t>玩家選擇的魔王</t>
-  </si>
-  <si>
     <t>下載魔王的prefab</t>
   </si>
   <si>
+    <t>string</t>
+  </si>
+  <si>
     <t>float</t>
-  </si>
-  <si>
-    <t>int</t>
-  </si>
-  <si>
-    <t>string</t>
   </si>
   <si>
     <t>Reaper</t>
@@ -103,12 +106,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF9900"/>
+        <bgColor rgb="FFFF9900"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -129,16 +138,27 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1"/>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="1" applyFont="1" fillId="2" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="1" applyFont="1" fillId="2" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" applyNumberFormat="1" fontId="1" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="2" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" applyNumberFormat="1" fontId="1" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="2" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1"/>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="1" applyFont="1" fillId="2" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+    <xf numFmtId="0" applyNumberFormat="1" fontId="2" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="1" applyFont="1" fillId="3" applyFill="1" borderId="0" applyBorder="1" xfId="0" applyProtection="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -348,13 +368,16 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:O4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col min="9" max="9" width="31.13" customWidth="1"/>
+    <col min="9" max="9" width="16" customWidth="1"/>
+    <col min="10" max="10" width="33.38" customWidth="1"/>
+    <col min="12" max="12" width="17.25" customWidth="1"/>
+    <col min="13" max="13" width="34.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -367,111 +390,131 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="J1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="3"/>
+      <c r="O1" s="4"/>
     </row>
     <row r="2">
       <c r="A2" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="C2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="D2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="E2" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="F2" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="G2" s="5" t="s">
         <v>16</v>
       </c>
+      <c r="H2" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="I2" s="3" t="s">
-        <v>17</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="K2" s="6"/>
+      <c r="O2" s="4"/>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="H3" s="3" t="s">
+      <c r="A3" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="B3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="J3" s="5" t="s">
         <v>20</v>
       </c>
+      <c r="K3" s="7"/>
+      <c r="O3" s="4"/>
     </row>
     <row r="4">
-      <c r="A4" s="1">
-        <v>2</v>
-      </c>
-      <c r="B4" s="1">
+      <c r="A4" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="5">
+        <v>12</v>
+      </c>
+      <c r="C4" s="3">
+        <v>200</v>
+      </c>
+      <c r="D4" s="3">
+        <v>3</v>
+      </c>
+      <c r="E4" s="3">
+        <v>1</v>
+      </c>
+      <c r="F4" s="3">
+        <v>1</v>
+      </c>
+      <c r="G4" s="3">
+        <v>5</v>
+      </c>
+      <c r="H4" s="3">
         <v>0</v>
       </c>
-      <c r="C4" s="1">
-        <v>1</v>
-      </c>
-      <c r="D4" s="1">
+      <c r="I4" s="3">
         <v>0</v>
       </c>
-      <c r="E4" s="1">
-        <v>0</v>
-      </c>
-      <c r="F4" s="1">
-        <v>1</v>
-      </c>
-      <c r="G4" s="1">
-        <v>0</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>22</v>
-      </c>
+      <c r="J4" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="K4" s="3"/>
+      <c r="O4" s="4"/>
     </row>
   </sheetData>
   <headerFooter/>

</xml_diff>

<commit_message>
update UI to suitable size
</commit_message>
<xml_diff>
--- a/MySurvivorsGame/Assets/StreamingAssets/RealTimePlayerData.xlsx
+++ b/MySurvivorsGame/Assets/StreamingAssets/RealTimePlayerData.xlsx
@@ -87,10 +87,10 @@
     <t>Reaper</t>
   </si>
   <si>
+    <t>0.899999976158142</t>
+  </si>
+  <si>
     <t>Assets/Prefabs/Devils/Reaper.prefab</t>
-  </si>
-  <si>
-    <t>MagicBall</t>
   </si>
 </sst>
 </file>
@@ -536,7 +536,7 @@
         <v>0</v>
       </c>
       <c r="J4" s="6">
-        <v>0.89999997615814209</v>
+        <v>0</v>
       </c>
       <c r="K4" s="10" t="s">
         <v>25</v>

</xml_diff>

<commit_message>
repair MagicBallController.cs sound bug
</commit_message>
<xml_diff>
--- a/MySurvivorsGame/Assets/StreamingAssets/RealTimePlayerData.xlsx
+++ b/MySurvivorsGame/Assets/StreamingAssets/RealTimePlayerData.xlsx
@@ -87,10 +87,10 @@
     <t>Reaper</t>
   </si>
   <si>
-    <t>0.899999976158142</t>
-  </si>
-  <si>
     <t>Assets/Prefabs/Devils/Reaper.prefab</t>
+  </si>
+  <si>
+    <t>MagicBall</t>
   </si>
 </sst>
 </file>
@@ -536,7 +536,7 @@
         <v>0</v>
       </c>
       <c r="J4" s="6">
-        <v>0</v>
+        <v>0.89999997615814209</v>
       </c>
       <c r="K4" s="10" t="s">
         <v>25</v>

</xml_diff>